<commit_message>
configuracion de solo escenarios exitoson en excel
configuracion para generar mensaje al momento que se presente un mensaje diferente a 200
</commit_message>
<xml_diff>
--- a/src/test/resources/data/users.xlsx
+++ b/src/test/resources/data/users.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="28">
   <si>
     <t>id</t>
   </si>
@@ -110,12 +110,6 @@
   </si>
   <si>
     <t>Kengor12</t>
-  </si>
-  <si>
-    <t>Kengor123</t>
-  </si>
-  <si>
-    <t>Kengor1234</t>
   </si>
 </sst>
 </file>
@@ -710,10 +704,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,28 +749,6 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>